<commit_message>
Second Commit for POM TestNG Framework....
</commit_message>
<xml_diff>
--- a/target/test-classes/com/tutorialninjaqa/testdata/TutorialsNinjaTestData.xlsx
+++ b/target/test-classes/com/tutorialninjaqa/testdata/TutorialsNinjaTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15915" windowHeight="7695"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
   <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>amotooricap9@gmail.com</t>
   </si>
   <si>
     <t>amotooricap1@gmail.com</t>
@@ -41,7 +38,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,53 +47,84 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -110,15 +138,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -128,6 +149,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,13 +176,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -163,38 +184,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,6 +206,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -227,13 +254,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,157 +386,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,8 +418,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -450,8 +456,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -472,17 +480,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,32 +512,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -544,150 +535,147 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1012,7 +1000,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1038,16 +1026,16 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>12345</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
+      <c r="A4" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>12345</v>
@@ -1057,6 +1045,7 @@
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="amotooricap1@gmail.com" tooltip="mailto:amotooricap1@gmail.com"/>
     <hyperlink ref="A4" r:id="rId2" display="amotooricap3@gmail.com" tooltip="mailto:amotooricap3@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="amotooricap1@gmail.com" tooltip="mailto:amotooricap1@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>